<commit_message>
working on reading Golden instances
</commit_message>
<xml_diff>
--- a/hw4_GA/Instances/BKS.xlsx
+++ b/hw4_GA/Instances/BKS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FDBEF2-2826-4549-8515-F64065F9CE03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="504" yWindow="1296" windowWidth="8064" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marc" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Marc</t>
   </si>
@@ -83,17 +84,41 @@
   </si>
   <si>
     <t>ρ = 75%</t>
+  </si>
+  <si>
+    <t>3500.7158</t>
+  </si>
+  <si>
+    <t>1986.89</t>
+  </si>
+  <si>
+    <t>2902.48</t>
+  </si>
+  <si>
+    <t>3215.310</t>
+  </si>
+  <si>
+    <t>3075.87</t>
+  </si>
+  <si>
+    <t>2251.90</t>
+  </si>
+  <si>
+    <t>2094.59</t>
+  </si>
+  <si>
+    <t>2730.05</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -101,13 +126,20 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -132,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -143,6 +175,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,25 +455,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.09765625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -448,96 +481,120 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>2016.57</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>1947.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>2602.56</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>2759.13</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>3028.83</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>2239.09</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>3343.34</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>3116.84</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working on bug fixing
</commit_message>
<xml_diff>
--- a/hw4_GA/Instances/BKS.xlsx
+++ b/hw4_GA/Instances/BKS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FDBEF2-2826-4549-8515-F64065F9CE03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6C27AA-7D45-4C4D-B352-36CCB6B1DB99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="504" yWindow="1296" windowWidth="8064" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="504" yWindow="1296" windowWidth="13056" windowHeight="10260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marc" sheetId="1" r:id="rId1"/>
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>